<commit_message>
Reg TCs for 811, 2805, 2648 stories
</commit_message>
<xml_diff>
--- a/Testdata/DataFile_ApplicationAccess_Check.xlsx
+++ b/Testdata/DataFile_ApplicationAccess_Check.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VersionControl\pse.autotest\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0491A47A-85F5-431F-B871-4E974C7CA6B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ADE6090-555F-475D-BD24-7D9B7D65E963}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="116">
   <si>
     <t>Population</t>
   </si>
@@ -365,6 +365,24 @@
   </si>
   <si>
     <t>Pfizer - RRMM_radio_button</t>
+  </si>
+  <si>
+    <t>NewImportLogic_2 - Test_Automation_2</t>
+  </si>
+  <si>
+    <t>NewImportLogic_2 - Test_Automation_2_radio_button</t>
+  </si>
+  <si>
+    <t>Usertype</t>
+  </si>
+  <si>
+    <t>Admin User</t>
+  </si>
+  <si>
+    <t>Staff User</t>
+  </si>
+  <si>
+    <t>Client User</t>
   </si>
 </sst>
 </file>
@@ -688,648 +706,661 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S31"/>
+  <dimension ref="A1:T31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="49.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="34.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="30.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="67" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="24.77734375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="27" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="24.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" customWidth="1"/>
+    <col min="3" max="3" width="31.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="49.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="34.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="67" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="24.77734375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="27" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="24.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>85</v>
       </c>
       <c r="B1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C1" t="s">
         <v>87</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>88</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>5</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>6</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>7</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>8</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>9</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>10</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>95</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>96</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>106</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>107</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>86</v>
       </c>
       <c r="B2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C2" t="s">
         <v>89</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>92</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>73</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>74</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>81</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>82</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>11</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>12</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>13</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>14</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>66</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>15</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>16</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>98</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>99</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>100</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>101</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>86</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>67</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>68</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>17</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>18</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>19</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>20</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>83</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>21</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>86</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>69</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>70</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>23</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>24</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>25</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>26</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>84</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>27</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>86</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>71</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>72</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>29</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>30</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>31</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>32</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>75</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>33</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="L6" t="s">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="M6" t="s">
         <v>76</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>35</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>93</v>
       </c>
       <c r="B7" t="s">
+        <v>114</v>
+      </c>
+      <c r="C7" t="s">
         <v>90</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>92</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>73</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>74</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>81</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>82</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>11</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>12</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>13</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>14</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>77</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>37</v>
       </c>
-      <c r="N7" t="s">
+      <c r="O7" t="s">
         <v>38</v>
       </c>
-      <c r="O7" t="s">
+      <c r="P7" t="s">
         <v>98</v>
       </c>
-      <c r="P7" t="s">
+      <c r="Q7" t="s">
         <v>99</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="R7" t="s">
         <v>100</v>
       </c>
-      <c r="R7" t="s">
+      <c r="S7" t="s">
         <v>101</v>
       </c>
-      <c r="S7" t="s">
+      <c r="T7" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>93</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>67</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>68</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>17</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>18</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>19</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>20</v>
       </c>
-      <c r="L8" t="s">
+      <c r="M8" t="s">
         <v>78</v>
       </c>
-      <c r="M8" t="s">
+      <c r="N8" t="s">
         <v>39</v>
       </c>
-      <c r="N8" t="s">
+      <c r="O8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>93</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>69</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>70</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>23</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>24</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>25</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>26</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
         <v>79</v>
       </c>
-      <c r="M9" t="s">
+      <c r="N9" t="s">
         <v>41</v>
       </c>
-      <c r="N9" t="s">
+      <c r="O9" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>93</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>71</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>72</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>29</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>30</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
         <v>31</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>32</v>
       </c>
-      <c r="L10" t="s">
+      <c r="M10" t="s">
         <v>80</v>
       </c>
-      <c r="M10" t="s">
+      <c r="N10" t="s">
         <v>43</v>
       </c>
-      <c r="N10" t="s">
+      <c r="O10" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="M11" t="s">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="N11" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>94</v>
       </c>
       <c r="B12" t="s">
+        <v>115</v>
+      </c>
+      <c r="C12" t="s">
         <v>91</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>92</v>
       </c>
-      <c r="D12" t="s">
-        <v>73</v>
-      </c>
       <c r="E12" t="s">
-        <v>74</v>
+        <v>110</v>
       </c>
       <c r="F12" t="s">
+        <v>111</v>
+      </c>
+      <c r="G12" t="s">
         <v>81</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>82</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>11</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>12</v>
       </c>
-      <c r="J12" t="s">
+      <c r="K12" t="s">
         <v>13</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>14</v>
       </c>
-      <c r="M12" t="s">
+      <c r="N12" t="s">
         <v>46</v>
       </c>
-      <c r="O12" t="s">
+      <c r="P12" t="s">
         <v>98</v>
       </c>
-      <c r="P12" t="s">
+      <c r="Q12" t="s">
         <v>99</v>
       </c>
-      <c r="Q12" t="s">
+      <c r="R12" t="s">
         <v>100</v>
       </c>
-      <c r="R12" t="s">
+      <c r="S12" t="s">
         <v>101</v>
       </c>
-      <c r="S12" t="s">
+      <c r="T12" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>94</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>108</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>109</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>67</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>68</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>17</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
         <v>18</v>
       </c>
-      <c r="J13" t="s">
+      <c r="K13" t="s">
         <v>19</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
         <v>20</v>
       </c>
-      <c r="M13" t="s">
+      <c r="N13" t="s">
         <v>47</v>
       </c>
-      <c r="O13" t="s">
+      <c r="P13" t="s">
         <v>103</v>
       </c>
-      <c r="P13" t="s">
+      <c r="Q13" t="s">
         <v>99</v>
       </c>
-      <c r="Q13" t="s">
+      <c r="R13" t="s">
         <v>104</v>
       </c>
-      <c r="R13" t="s">
+      <c r="S13" t="s">
         <v>101</v>
       </c>
-      <c r="S13" t="s">
+      <c r="T13" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>94</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>69</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>70</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I14" t="s">
         <v>23</v>
       </c>
-      <c r="I14" t="s">
+      <c r="J14" t="s">
         <v>24</v>
       </c>
-      <c r="J14" t="s">
+      <c r="K14" t="s">
         <v>25</v>
       </c>
-      <c r="K14" t="s">
+      <c r="L14" t="s">
         <v>26</v>
       </c>
-      <c r="M14" t="s">
+      <c r="N14" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>94</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>71</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
         <v>72</v>
       </c>
-      <c r="H15" t="s">
+      <c r="I15" t="s">
         <v>29</v>
       </c>
-      <c r="I15" t="s">
+      <c r="J15" t="s">
         <v>30</v>
       </c>
-      <c r="J15" t="s">
+      <c r="K15" t="s">
         <v>31</v>
       </c>
-      <c r="K15" t="s">
+      <c r="L15" t="s">
         <v>32</v>
       </c>
-      <c r="M15" t="s">
+      <c r="N15" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="M16" t="s">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="N16" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="13:13" x14ac:dyDescent="0.3">
-      <c r="M17" t="s">
+    <row r="17" spans="14:14" x14ac:dyDescent="0.3">
+      <c r="N17" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="13:13" x14ac:dyDescent="0.3">
-      <c r="M18" t="s">
+    <row r="18" spans="14:14" x14ac:dyDescent="0.3">
+      <c r="N18" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="13:13" x14ac:dyDescent="0.3">
-      <c r="M19" t="s">
+    <row r="19" spans="14:14" x14ac:dyDescent="0.3">
+      <c r="N19" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="13:13" x14ac:dyDescent="0.3">
-      <c r="M20" t="s">
+    <row r="20" spans="14:14" x14ac:dyDescent="0.3">
+      <c r="N20" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="13:13" x14ac:dyDescent="0.3">
-      <c r="M21" t="s">
+    <row r="21" spans="14:14" x14ac:dyDescent="0.3">
+      <c r="N21" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="22" spans="13:13" x14ac:dyDescent="0.3">
-      <c r="M22" t="s">
+    <row r="22" spans="14:14" x14ac:dyDescent="0.3">
+      <c r="N22" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="13:13" x14ac:dyDescent="0.3">
-      <c r="M23" t="s">
+    <row r="23" spans="14:14" x14ac:dyDescent="0.3">
+      <c r="N23" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="13:13" x14ac:dyDescent="0.3">
-      <c r="M24" t="s">
+    <row r="24" spans="14:14" x14ac:dyDescent="0.3">
+      <c r="N24" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="25" spans="13:13" x14ac:dyDescent="0.3">
-      <c r="M25" t="s">
+    <row r="25" spans="14:14" x14ac:dyDescent="0.3">
+      <c r="N25" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="26" spans="13:13" x14ac:dyDescent="0.3">
-      <c r="M26" t="s">
+    <row r="26" spans="14:14" x14ac:dyDescent="0.3">
+      <c r="N26" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="13:13" x14ac:dyDescent="0.3">
-      <c r="M27" t="s">
+    <row r="27" spans="14:14" x14ac:dyDescent="0.3">
+      <c r="N27" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="28" spans="13:13" x14ac:dyDescent="0.3">
-      <c r="M28" t="s">
+    <row r="28" spans="14:14" x14ac:dyDescent="0.3">
+      <c r="N28" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="13:13" x14ac:dyDescent="0.3">
-      <c r="M29" t="s">
+    <row r="29" spans="14:14" x14ac:dyDescent="0.3">
+      <c r="N29" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="30" spans="13:13" x14ac:dyDescent="0.3">
-      <c r="M30" t="s">
+    <row r="30" spans="14:14" x14ac:dyDescent="0.3">
+      <c r="N30" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="31" spans="13:13" x14ac:dyDescent="0.3">
-      <c r="M31" t="s">
+    <row r="31" spans="14:14" x14ac:dyDescent="0.3">
+      <c r="N31" t="s">
         <v>65</v>
       </c>
     </row>

</xml_diff>